<commit_message>
alter citationGraph and Matrix
</commit_message>
<xml_diff>
--- a/experiments/experiment_1/notebooks/tabela_grafo.xlsx
+++ b/experiments/experiment_1/notebooks/tabela_grafo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="361">
   <si>
     <t>S</t>
   </si>
@@ -460,7 +460,7 @@
     <t>basili1984a, basili1989a, basili1994a, becker1999a, bianchi2001a, buglione2000a, card2003b, chrissis2003a, cobit2007a, kaplan1992a, offen1997a, ogc2002a, usddusa2003a, weiss1998a, basili1994b</t>
   </si>
   <si>
-    <t>mandić2010b, accenture2004a, sw1998a, ai1994a, basili1981a, basili1985a, basili1989a, basili1993a, basili1995b, basili1994e, basili1988c, basili1984b, basili1994f, basili1994a, basili1995a, basili1996a, basili2010a, beck2004a, becker1999a, boehm2003b, briand1996a, brindgeland2008a, budd2009a, buglione2000a, burlton2010a, chillarege1992a, ciolkowski2002a, cmmi2010a, conradi2002a, damiani2008a, deming1986b, eckerson2005a, epstein1998a, fagan1976b, gamma1994a, gartner2010a, gartner2011a, gresse1995a, hammer1990b, hammer2010a, hammer1993a, humphrey2005a, isoiec2009a, kaplan1992a, kaplan1996a, kaplan2004b, kaplan2008b, kerth2001a, laitenberger2002a, (2012, Mandić, Vladimir), mandić2010a, mandić2010g, mandić2010b, nch2004a, unch2012a, neely1995a, nudurupati2011a, offen1997a, ogc2009a, omg2010a, pmi2013a, porter1996a, porter2008a, rombach1995a, rosemann2010a, sarcia2010a, schwaber2004a, selby2005a, shewhart1939a, trendowicz2011a, solingen1999b</t>
+    <t>mandić2010b, accenture2004a, sw1998a, ai1994a, basili1981a, basili1985a, basili1989a, basili1993a, basili1995b, basili1994e, basili1988c, basili1984b, basili1994f, basili1994a, basili1995a, basili1996a, basili2010a, beck2004a, becker1999a, boehm2003b, briand1996a, brindgeland2008a, budd2009a, buglione2000a, burlton2010a, chillarege1992a, ciolkowski2002a, cmmi2010a, conradi2002a, damiani2008a, deming1986b, eckerson2005a, epstein1998a, fagan1976b, gamma1994a, gartner2010a, gartner2011a, gresse1995a, hammer1990b, hammer2010a, hammer1993a, humphrey2005a, isoiec2009a, kaplan1992a, kaplan1996a, kaplan2004b, kaplan2008b, kerth2001a, laitenberger2002a, mandic2012a, mandić2010a, mandić2010g, mandić2010b, nch2004a, unch2012a, neely1995a, nudurupati2011a, offen1997a, ogc2009a, omg2010a, pmi2013a, porter1996a, porter2008a, rombach1995a, rosemann2010a, sarcia2010a, schwaber2004a, selby2005a, shewhart1939a, trendowicz2011a, solingen1999b</t>
   </si>
   <si>
     <t>mandić2010b, pfeffer1998a, staron2011a, basili2010a, basili1994a, basili1994b, mandić2010b, lyne2003a, peppard2001a, rautiainen1999a, krishnan2001a, curtis1988a, dagnino2001a, jaufman2004a, karlström2005b, genus2006a, dove2005a, patanakul2010a, turner2007a, allee2008a, mcgrath2004a, sicotte2000a, lainhart2000a, mcgarry2002a, kaplan1992a, pan2007a, olsina2011b, papa2012a, mandić2010c, kowalczyk2010a, edmondson2007a, gummesson1991a</t>
@@ -586,7 +586,7 @@
     <t>lepmets2012a, becker2012a, pryor2011a, vasconcellos2017a, dadhich2012a, barreto2011a, cyrus2011a, lópez2012a, ramos2015a, sanchez2017a, mitre2014a, hamouda2013a, sanchez2018a, haghighatfar2013a, valenciennes2013a, aguirre2014a, mitrehernández2014a, salgado2015a, robles2016a</t>
   </si>
   <si>
-    <t>buse2012a, wallace2014a, paternoster2014a, novais2013a, lew2012a, giardino2014a, kim2016a, trendowicz2013a, guzmán2010a, papa2012a, sarcia2010a, bird2015a, becker2012a, basili2013a, becker2015a, becker2011b, olsina2011a, lew2011a, gencel2013a, mandić2010c, cedergren2011a, kläs2015a, olsina2014a, ferreira2013a, münch2012a, kobori2014b, monden2012a, olsina2011b, rivera2016a, kläs2013a, kobori2014a, liggesmeyer2014a, rivera2016b, giannoulis2013a, tahir2016a, álvarez2015a, heidrich2014a, murphy2015a, eremenko2012a, cedergren2014a, aoki2016a, jedlitschka2013a, mandić2010f, jahn2014a, lescher2011a, kobori2016a, zhang2014a, oberscheven2013a, lavazza2011a, giannoulis2014a, djouab2016a, hernández2010a, hästbacka2013a, leschera2012a, guinea2013a, lópez2016b, janes2014a, osadchyy2013a, khalifa2016a, lópez2016a, ahmad2016a, papa2016a, kettunen2014a, mandić2017a, ebner2014a, lavazza2013a, heidrich2013a, koumaditis2015a, marca2010a, sanchez2017a, poligadu2014a, koumaditis2016a, jaramillo2016a, rivera2015a, heidrich2012a, doerr2013a, novais2018a, asghari2012a, olsina2017a, lavazza2015a, washizaki2017a, pérez2017a, becker2014a, papa2012b, papa2015a, rivera2015b, rivera2016c, becker2017a, basili2014a, yamamoto2016a, falessi2014a, diep2016a, mitre2014a, machado2012a, abdulameer2015a, (2012, Mandić, Vladimir), rombach2014a, port2016a, santos2017a, olsina2013a, armstrong2016a, cedergren2011b, anders9999a, sanchez2018a, machado2016a, heidrich9999a, zapata2017a, mughal2017a, lavazza2015b, nicho2017a, mitrehernández2014a, olsina2012b, jørgensen2014a, hästbacka2013b, trendowicz2014b, hyvönen2015a, rombach2012a, eremenko2013a, erukulapati2017a, jeners2015a, rensburg2012a, boehm2014a, pinheiro2017a, mandić2012b, ferreira2014a, tebes2017a, xu2015a, trendowicz9999a, lang2014a, lang2017a, papa9999a, lang2017b, huberts9999a, mendoza2013a, robles2016a, cocozza2014a, mandić2010a, mandić2010b, mandić2010d, münch2013a, münch2013c, petersen2015a, trendowicz2011a, trendowicz2014a, unterkalmsteiner2014a</t>
+    <t>buse2012a, wallace2014a, paternoster2014a, novais2013a, lew2012a, giardino2014a, kim2016a, trendowicz2013a, guzmán2010a, papa2012a, sarcia2010a, bird2015a, becker2012a, basili2013a, becker2015a, becker2011b, olsina2011a, lew2011a, gencel2013a, mandić2010c, cedergren2011a, kläs2015a, olsina2014a, ferreira2013a, münch2012a, kobori2014b, monden2012a, olsina2011b, rivera2016a, kläs2013a, kobori2014a, liggesmeyer2014a, rivera2016b, giannoulis2013a, tahir2016a, álvarez2015a, heidrich2014a, murphy2015a, eremenko2012a, cedergren2014a, aoki2016a, jedlitschka2013a, mandić2010f, jahn2014a, lescher2011a, kobori2016a, zhang2014a, oberscheven2013a, lavazza2011a, giannoulis2014a, djouab2016a, hernández2010a, hästbacka2013a, leschera2012a, guinea2013a, lópez2016b, janes2014a, osadchyy2013a, khalifa2016a, lópez2016a, ahmad2016a, papa2016a, kettunen2014a, mandić2017a, ebner2014a, lavazza2013a, heidrich2013a, koumaditis2015a, marca2010a, sanchez2017a, poligadu2014a, koumaditis2016a, jaramillo2016a, rivera2015a, heidrich2012a, doerr2013a, novais2018a, asghari2012a, olsina2017a, lavazza2015a, washizaki2017a, pérez2017a, becker2014a, papa2012b, papa2015a, rivera2015b, rivera2016c, becker2017a, basili2014a, yamamoto2016a, falessi2014a, diep2016a, mitre2014a, machado2012a, abdulameer2015a, mandic2012a, rombach2014a, port2016a, santos2017a, olsina2013a, armstrong2016a, cedergren2011b, anders9999a, sanchez2018a, machado2016a, heidrich9999a, zapata2017a, mughal2017a, lavazza2015b, nicho2017a, mitrehernández2014a, olsina2012b, jørgensen2014a, hästbacka2013b, trendowicz2014b, hyvönen2015a, rombach2012a, eremenko2013a, erukulapati2017a, jeners2015a, rensburg2012a, boehm2014a, pinheiro2017a, mandić2012b, ferreira2014a, tebes2017a, xu2015a, trendowicz9999a, lang2014a, lang2017a, papa9999a, lang2017b, huberts9999a, mendoza2013a, robles2016a, cocozza2014a, mandić2010a, mandić2010b, mandić2010d, münch2013a, münch2013c, petersen2015a, trendowicz2011a, trendowicz2014a, unterkalmsteiner2014a</t>
   </si>
   <si>
     <t>karlström2002a, marcus2005a, kandé2000a, sawyer2002a, liu2008a, katz2004a, ghose2007a, gans2003a, karlström2005a, ghose2007b, kabbaj2008a, egorova2009a, marcelloni2001a, easterbrook2001a, yang2007a, zhang2009a, acharya2005a, nguyen2003a, taipale2007a, rayson1999a, rayson2000a, katz2004b, rayson1999b, bent2006a, kim2014a, rayson1999c, soares2012a, zhang2010a, nguyen2004a, müller2012a, eljabiri2012a, michel2009a, aysolmaz2011a, eljabiri2001a, berkovich2012a, nunn2016a, morisio2009a, aida2003a, charrel2007a, jun2007a, jurczuk2017b, jesko9999a, solaimani2017a, jurczuk2017a, karlström2002b, lui2008a, nair2009a, francalanci2016a, ghose9999a, solaimani2014a, zhiping2011a, alves2002a, vázquez2001a, vazquez2000a, apfelbacher2007a</t>
@@ -667,7 +667,7 @@
     <t>becker2008a, becker2008b</t>
   </si>
   <si>
-    <t>basili2009a, damiani2008a, aversano2016a, mandić2010c, ellis2012a, mulazzani2009a, samtani2012a, kelanti2013a, álvarez2015a, samtani2012b, quintero2012a, aoki2016a, mandić2010f, ellis2013a, heidrich2009a, hyysalo2014a, münch2012b, kobori2016a, münch2012c, ellis2013b, texel2015a, molina2012a, münch2009a, ahmad2016a, texel2013a, mandić2017a, mulazzani2009b, aoki2017a, roditi2014a, asghari2012a, pérez2017a, becker2014a, papa2015a, aarts2016a, cahyaningsih2014a, jayatilleke2017a, (2012, Mandić, Vladimir), lindqvist2016a, mughal2017a, kramer2014a, mulazzani2009c, monden2017a, nagel2015a, casare2012a, cervantes2016a, cervantes2012a, santo2015a, aarts2016a, chaos9999a, pinto9999a, basili2010a, cocozza2014a, mandić2010b, mandić2010d, petersen2015a</t>
+    <t>basili2009a, damiani2008a, aversano2016a, mandić2010c, ellis2012a, mulazzani2009a, samtani2012a, kelanti2013a, álvarez2015a, samtani2012b, quintero2012a, aoki2016a, mandić2010f, ellis2013a, heidrich2009a, hyysalo2014a, münch2012b, kobori2016a, münch2012c, ellis2013b, texel2015a, molina2012a, münch2009a, ahmad2016a, texel2013a, mandić2017a, mulazzani2009b, aoki2017a, roditi2014a, asghari2012a, pérez2017a, becker2014a, papa2015a, aarts2016a, cahyaningsih2014a, jayatilleke2017a, mandic2012a, lindqvist2016a, mughal2017a, kramer2014a, mulazzani2009c, monden2017a, nagel2015a, casare2012a, cervantes2016a, cervantes2012a, santo2015a, aarts2016a, chaos9999a, pinto9999a, basili2010a, cocozza2014a, mandić2010b, mandić2010d, petersen2015a</t>
   </si>
   <si>
     <t>oliveira2018a</t>
@@ -679,7 +679,7 @@
     <t>lópez2016a, mandić2017a, hooge2016a, trinkenreich2017b, chagas2016a, petersen2015a</t>
   </si>
   <si>
-    <t>barreto2010a, münch2013e, amannejad2014a, sarcia2010a, harjumaa2008a, damiani2008a, ramler2010a, mandić2010c, caputo2010a, umarji2009b, kowalczyk2014a, danovaro2008a, fabijan2016a, cedergren2014a, yang2010a, przybylek2011a, uchida2016a, mandić2010f, buglione2011a, garousi2012a, barreto2009a, bennicke2008a, kowalczyk2013a, thammarak2011a, hernández2010a, guinea2013a, janes2014a, münch2009a, mandić2010e, mandić2017a, heidrich2012a, teles2014a, armbrust2007a, júnior2010a, mitre2014a, tsunoda2011a, (2012, Mandić, Vladimir), marcos2017a, watanabe2017a, janes2014b, machado2016a, ferreira2018a, thammarak2013a, mitrehernández2014a, moraes2017a, katopodis2015a, debruyn2014a, ferreira2014a, cansado2012a, bóka2009a, trinkenreich2015b, montebelo2008a, pimentel2016a, pinho2010a, dashkov2017a, rocha2009a, papazov9999a, cansado9999a, voigt9999a, marcos2017b, trinkenreich2015b, pimentel2016a, pinto9999a, rivera9999a, rocha2009a, kaneko2011a, kowalczyk2010a, mandić2010b, unterkalmsteiner2014a</t>
+    <t>barreto2010a, münch2013e, amannejad2014a, sarcia2010a, harjumaa2008a, damiani2008a, ramler2010a, mandić2010c, caputo2010a, umarji2009b, kowalczyk2014a, danovaro2008a, fabijan2016a, cedergren2014a, yang2010a, przybylek2011a, uchida2016a, mandić2010f, buglione2011a, garousi2012a, barreto2009a, bennicke2008a, kowalczyk2013a, thammarak2011a, hernández2010a, guinea2013a, janes2014a, münch2009a, mandić2010e, mandić2017a, heidrich2012a, teles2014a, armbrust2007a, júnior2010a, mitre2014a, tsunoda2011a, mandic2012a, marcos2017a, watanabe2017a, janes2014b, machado2016a, ferreira2018a, thammarak2013a, mitrehernández2014a, moraes2017a, katopodis2015a, debruyn2014a, ferreira2014a, cansado2012a, bóka2009a, trinkenreich2015b, montebelo2008a, pimentel2016a, pinho2010a, dashkov2017a, rocha2009a, papazov9999a, cansado9999a, voigt9999a, marcos2017b, trinkenreich2015b, pimentel2016a, pinto9999a, rivera9999a, rocha2009a, kaneko2011a, kowalczyk2010a, mandić2010b, unterkalmsteiner2014a</t>
   </si>
   <si>
     <t>petersen2015a, basili2014b, monden2012a, kobori2014a, shimura2017a, alves2014a, ellis2013a, kobori2016a, lópez2016a, mandić2017a, jaramillo2016a, heidrich2012a, asghari2012a, zapata2017a, brehm2014a, trendowicz2014a</t>
@@ -703,7 +703,7 @@
     <t>kwak2006a, aboelmaged2010a, unterkalmsteiner2012a, subramanian2007a, nonthaleerak2006a, wu2006a, tjahjono2010a, tang2007a, mahanti2005a, anbari2004a, siviy2007a, mahanti2009a, kundu2012a, wang2005b, mahanti2006a, jiang2011a, knowles2011a, brady2005a, garcia2009a, antoniol2004a, kundu2012b, patel2009a, li2008a, patyal2015a, bahli2004a, zhang2008c, landaeta2008a, asato2011a, bubevski2014a, müller2012a, besseris2010a, kundu2016a, cheng2009a, wandersman2012a, rico2010a, el2011a, barcellos2008b, el2013a, unterkalmsteiner2010a, wang2005c, chen2007b, deng2015a, daubner2008a, rico9999a, choi2006a, khan2016a, dalipi2012a, nyambegera2014a, islam2009a, strate2013a, el2010b, zhang9999a, tong2009a, paruchuri2009a, manohar9999a, manohar9999a, sharma2012a, tse2005a, bubevski2016a, u2018a, chen2007c, al2018a, sharma2017a, simmons2010a, mahanti2014a, cerdeiral2017a, quintella2017a, barcellos9999a, mayoral2012a, andrade9999a, sun2012a, tonini2006a, quintella9999a, caivano9999a, horizonte2017a, unterkalmsteiner2014a, wang2005a</t>
   </si>
   <si>
-    <t>fagerholm2014a, mandić2010b, fagerholm2017a, lindgren2015a, heidrich2008a, papa2012a, lindgren2016a, mandić2010d, olsina2011b, luo2016a, kowalczyk2014a, dumke2009a, mandić2010f, ta2015a, münch2012b, kelemen2014a, dumke2014a, dumke2013a, münch2009a, valle2017a, papa2016a, heidrich2010a, luo2015a, roditi2014a, ciolkowski2008a, becker2014a, papa2012b, papa2015a, (2012, Mandić, Vladimir), cuadrado2010a, sadabadi2016a, sakul2017a, lindgren2015b, kowalczyk2010a, münch2013a</t>
+    <t>fagerholm2014a, mandić2010b, fagerholm2017a, lindgren2015a, heidrich2008a, papa2012a, lindgren2016a, mandić2010d, olsina2011b, luo2016a, kowalczyk2014a, dumke2009a, mandić2010f, ta2015a, münch2012b, kelemen2014a, dumke2014a, dumke2013a, münch2009a, valle2017a, papa2016a, heidrich2010a, luo2015a, roditi2014a, ciolkowski2008a, becker2014a, papa2012b, papa2015a, mandic2012a, cuadrado2010a, sadabadi2016a, sakul2017a, lindgren2015b, kowalczyk2010a, münch2013a</t>
   </si>
   <si>
     <t>selected forward list</t>
@@ -1097,15 +1097,6 @@
   </si>
   <si>
     <t>Step 8</t>
-  </si>
-  <si>
-    <t>becker2008a, trienekens2009a</t>
-  </si>
-  <si>
-    <t>becker2008a, trienekens2009a, birkhölzer2011a</t>
-  </si>
-  <si>
-    <t>trienekens2009a, birkhölzer2011a</t>
   </si>
 </sst>
 </file>
@@ -1630,9 +1621,6 @@
       <c r="L3" t="s">
         <v>182</v>
       </c>
-      <c r="U3" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="4" spans="1:21">
       <c r="A4" s="1">
@@ -1668,9 +1656,6 @@
       <c r="L4" t="s">
         <v>183</v>
       </c>
-      <c r="U4" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="5" spans="1:21">
       <c r="A5" s="1">
@@ -1731,7 +1716,7 @@
         <v>357</v>
       </c>
       <c r="U5" t="s">
-        <v>361</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -1789,9 +1774,6 @@
       <c r="S6" t="s">
         <v>350</v>
       </c>
-      <c r="U6" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="7" spans="1:21">
       <c r="A7" s="1">
@@ -1848,9 +1830,6 @@
       <c r="R7" t="s">
         <v>347</v>
       </c>
-      <c r="U7" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" s="1">
@@ -1904,9 +1883,6 @@
       <c r="R8" t="s">
         <v>348</v>
       </c>
-      <c r="U8" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="9" spans="1:21">
       <c r="A9" s="1">
@@ -1967,7 +1943,7 @@
         <v>338</v>
       </c>
       <c r="U9" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -2028,9 +2004,6 @@
       <c r="T10" t="s">
         <v>350</v>
       </c>
-      <c r="U10" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="11" spans="1:21">
       <c r="A11" s="1">
@@ -2090,9 +2063,6 @@
       <c r="S11" t="s">
         <v>350</v>
       </c>
-      <c r="U11" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="1">
@@ -2134,9 +2104,6 @@
       <c r="N12" t="s">
         <v>79</v>
       </c>
-      <c r="U12" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="1">
@@ -2196,9 +2163,6 @@
       <c r="T13" t="s">
         <v>350</v>
       </c>
-      <c r="U13" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="14" spans="1:21">
       <c r="A14" s="1">
@@ -2243,9 +2207,6 @@
       <c r="O14" t="s">
         <v>66</v>
       </c>
-      <c r="U14" t="s">
-        <v>64</v>
-      </c>
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="1">
@@ -2287,9 +2248,6 @@
       <c r="N15" t="s">
         <v>80</v>
       </c>
-      <c r="U15" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="1">
@@ -2334,11 +2292,8 @@
       <c r="O16" t="s">
         <v>64</v>
       </c>
-      <c r="U16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21">
+    </row>
+    <row r="17" spans="1:20">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2378,11 +2333,8 @@
       <c r="N17" t="s">
         <v>81</v>
       </c>
-      <c r="U17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21">
+    </row>
+    <row r="18" spans="1:20">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2440,11 +2392,8 @@
       <c r="S18" t="s">
         <v>350</v>
       </c>
-      <c r="U18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21">
+    </row>
+    <row r="19" spans="1:20">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2502,11 +2451,8 @@
       <c r="T19" t="s">
         <v>99</v>
       </c>
-      <c r="U19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21">
+    </row>
+    <row r="20" spans="1:20">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2540,11 +2486,8 @@
       <c r="L20" t="s">
         <v>199</v>
       </c>
-      <c r="U20" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21">
+    </row>
+    <row r="21" spans="1:20">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2602,11 +2545,8 @@
       <c r="S21" t="s">
         <v>59</v>
       </c>
-      <c r="U21" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21">
+    </row>
+    <row r="22" spans="1:20">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2646,11 +2586,8 @@
       <c r="N22" t="s">
         <v>85</v>
       </c>
-      <c r="U22" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21">
+    </row>
+    <row r="23" spans="1:20">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2684,11 +2621,8 @@
       <c r="L23" t="s">
         <v>202</v>
       </c>
-      <c r="U23" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21">
+    </row>
+    <row r="24" spans="1:20">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2743,11 +2677,8 @@
       <c r="R24" t="s">
         <v>347</v>
       </c>
-      <c r="U24" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21">
+    </row>
+    <row r="25" spans="1:20">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2802,11 +2733,8 @@
       <c r="T25" t="s">
         <v>59</v>
       </c>
-      <c r="U25" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21">
+    </row>
+    <row r="26" spans="1:20">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2867,11 +2795,8 @@
       <c r="T26" t="s">
         <v>350</v>
       </c>
-      <c r="U26" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21">
+    </row>
+    <row r="27" spans="1:20">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2926,11 +2851,8 @@
       <c r="S27" t="s">
         <v>350</v>
       </c>
-      <c r="U27" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21">
+    </row>
+    <row r="28" spans="1:20">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2982,11 +2904,8 @@
       <c r="R28" t="s">
         <v>350</v>
       </c>
-      <c r="U28" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21">
+    </row>
+    <row r="29" spans="1:20">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -3026,11 +2945,8 @@
       <c r="N29" t="s">
         <v>62</v>
       </c>
-      <c r="U29" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21">
+    </row>
+    <row r="30" spans="1:20">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -3067,11 +2983,8 @@
       <c r="N30" t="s">
         <v>65</v>
       </c>
-      <c r="U30" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21">
+    </row>
+    <row r="31" spans="1:20">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -3111,11 +3024,8 @@
       <c r="N31" t="s">
         <v>67</v>
       </c>
-      <c r="U31" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21">
+    </row>
+    <row r="32" spans="1:20">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -3173,11 +3083,8 @@
       <c r="T32" t="s">
         <v>59</v>
       </c>
-      <c r="U32" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21">
+    </row>
+    <row r="33" spans="1:20">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -3238,11 +3145,8 @@
       <c r="T33" t="s">
         <v>59</v>
       </c>
-      <c r="U33" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21">
+    </row>
+    <row r="34" spans="1:20">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -3297,11 +3201,8 @@
       <c r="S34" t="s">
         <v>99</v>
       </c>
-      <c r="U34" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21">
+    </row>
+    <row r="35" spans="1:20">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -3341,11 +3242,8 @@
       <c r="N35" t="s">
         <v>72</v>
       </c>
-      <c r="U35" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21">
+    </row>
+    <row r="36" spans="1:20">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -3400,11 +3298,8 @@
       <c r="R36" t="s">
         <v>353</v>
       </c>
-      <c r="U36" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21">
+    </row>
+    <row r="37" spans="1:20">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -3459,11 +3354,8 @@
       <c r="S37" t="s">
         <v>353</v>
       </c>
-      <c r="U37" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21">
+    </row>
+    <row r="38" spans="1:20">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -3521,11 +3413,8 @@
       <c r="T38" t="s">
         <v>59</v>
       </c>
-      <c r="U38" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21">
+    </row>
+    <row r="39" spans="1:20">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -3583,11 +3472,8 @@
       <c r="T39" t="s">
         <v>59</v>
       </c>
-      <c r="U39" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21">
+    </row>
+    <row r="40" spans="1:20">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -3642,11 +3528,8 @@
       <c r="S40" t="s">
         <v>350</v>
       </c>
-      <c r="U40" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21">
+    </row>
+    <row r="41" spans="1:20">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -3701,11 +3584,8 @@
       <c r="S41" t="s">
         <v>350</v>
       </c>
-      <c r="U41" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21">
+    </row>
+    <row r="42" spans="1:20">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -3763,11 +3643,8 @@
       <c r="S42" t="s">
         <v>350</v>
       </c>
-      <c r="U42" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21">
+    </row>
+    <row r="43" spans="1:20">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -3828,11 +3705,8 @@
       <c r="T43" t="s">
         <v>350</v>
       </c>
-      <c r="U43" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21">
+    </row>
+    <row r="44" spans="1:20">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -3881,11 +3755,8 @@
       <c r="Q44" t="s">
         <v>343</v>
       </c>
-      <c r="U44" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21">
+    </row>
+    <row r="45" spans="1:20">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -3946,11 +3817,8 @@
       <c r="T45" t="s">
         <v>350</v>
       </c>
-      <c r="U45" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21">
+    </row>
+    <row r="46" spans="1:20">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -3990,11 +3858,8 @@
       <c r="N46" t="s">
         <v>268</v>
       </c>
-      <c r="U46" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21">
+    </row>
+    <row r="47" spans="1:20">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -4049,11 +3914,8 @@
       <c r="T47" t="s">
         <v>59</v>
       </c>
-      <c r="U47" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21">
+    </row>
+    <row r="48" spans="1:20">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -4107,9 +3969,6 @@
       </c>
       <c r="S48" t="s">
         <v>358</v>
-      </c>
-      <c r="U48" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="49" spans="1:21">
@@ -4171,7 +4030,7 @@
         <v>349</v>
       </c>
       <c r="U49" t="s">
-        <v>363</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50" spans="1:21">
@@ -4232,9 +4091,6 @@
       <c r="T50" t="s">
         <v>99</v>
       </c>
-      <c r="U50" t="s">
-        <v>100</v>
-      </c>
     </row>
     <row r="51" spans="1:21">
       <c r="A51" s="1">
@@ -4291,9 +4147,6 @@
       <c r="R51" t="s">
         <v>347</v>
       </c>
-      <c r="U51" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="52" spans="1:21">
       <c r="A52" s="1">
@@ -4350,9 +4203,6 @@
       <c r="S52" t="s">
         <v>350</v>
       </c>
-      <c r="U52" t="s">
-        <v>102</v>
-      </c>
     </row>
     <row r="53" spans="1:21">
       <c r="A53" s="1">
@@ -4408,9 +4258,6 @@
       </c>
       <c r="S53" t="s">
         <v>347</v>
-      </c>
-      <c r="U53" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>